<commit_message>
student times match expect output now as well
</commit_message>
<xml_diff>
--- a/final_project/testing/shared_data/student_test_expected_output.xlsx
+++ b/final_project/testing/shared_data/student_test_expected_output.xlsx
@@ -14,13 +14,13 @@
   <sheets>
     <sheet name="student_test_expected_output" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +155,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF303030"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,8 +354,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -464,6 +476,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -509,11 +536,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="18" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -835,264 +869,563 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>100000005</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="1">
+        <v>100000066</v>
+      </c>
+      <c r="E1" s="3">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1">
+        <v>100000005</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4">
+        <v>100000005</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="M1" s="5">
+        <v>100000005</v>
+      </c>
+      <c r="N1" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>100000066</v>
+      </c>
+      <c r="E2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>100000066</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
+        <v>100000066</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5">
+        <v>100000066</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100000066</v>
       </c>
       <c r="D3" s="1">
+        <v>100002460</v>
+      </c>
+      <c r="E3" s="3">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100002460</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="J3" s="4">
         <v>100000066</v>
       </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="M3" s="5">
+        <v>100000066</v>
+      </c>
+      <c r="N3" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>100000066</v>
+        <v>100003192</v>
       </c>
       <c r="E4" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>100003192</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4">
+        <v>100002460</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="M4" s="5">
+        <v>100002460</v>
+      </c>
+      <c r="N4" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100000066</v>
       </c>
       <c r="D5" s="1">
-        <v>100002460</v>
+        <v>100003268</v>
       </c>
       <c r="E5" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1">
+        <v>100003268</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="J5" s="4">
+        <v>100003192</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="M5" s="5">
+        <v>100003192</v>
+      </c>
+      <c r="N5" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>100003192</v>
+        <v>100004467</v>
       </c>
       <c r="E6" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1">
+        <v>100004467</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="J6" s="4">
+        <v>100003268</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="M6" s="5">
+        <v>100003268</v>
+      </c>
+      <c r="N6" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100002460</v>
       </c>
       <c r="D7" s="1">
-        <v>100003268</v>
+        <v>100004467</v>
       </c>
       <c r="E7" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1">
+        <v>100004819</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="J7" s="4">
+        <v>100004467</v>
+      </c>
+      <c r="K7">
+        <v>12</v>
+      </c>
+      <c r="M7" s="5">
+        <v>100004467</v>
+      </c>
+      <c r="N7" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>12</v>
       </c>
       <c r="D8" s="1">
+        <v>100004819</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>100005156</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
+      </c>
+      <c r="J8" s="4">
         <v>100004467</v>
       </c>
-      <c r="E8" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="M8" s="5">
+        <v>100004467</v>
+      </c>
+      <c r="N8" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>100003192</v>
       </c>
       <c r="D9" s="1">
-        <v>100004467</v>
+        <v>100005156</v>
       </c>
       <c r="E9" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1">
+        <v>100007808</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="J9" s="4">
+        <v>100004819</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="M9" s="5">
+        <v>100004819</v>
+      </c>
+      <c r="N9" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>100004819</v>
+        <v>100007808</v>
       </c>
       <c r="E10" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1">
+        <v>100008254</v>
+      </c>
+      <c r="H10">
+        <v>22</v>
+      </c>
+      <c r="J10" s="4">
+        <v>100005156</v>
+      </c>
+      <c r="K10">
+        <v>17</v>
+      </c>
+      <c r="M10" s="5">
+        <v>100005156</v>
+      </c>
+      <c r="N10" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>100003268</v>
       </c>
       <c r="D11" s="1">
-        <v>100005156</v>
+        <v>100008254</v>
       </c>
       <c r="E11" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="G11" s="1">
+        <v>100010128</v>
+      </c>
+      <c r="H11">
+        <v>14</v>
+      </c>
+      <c r="J11" s="4">
+        <v>100007808</v>
+      </c>
+      <c r="K11">
+        <v>12</v>
+      </c>
+      <c r="M11" s="5">
+        <v>100007808</v>
+      </c>
+      <c r="N11" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>15</v>
       </c>
       <c r="D12" s="1">
-        <v>100007808</v>
+        <v>100010128</v>
       </c>
       <c r="E12" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1">
+        <v>100012200</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="J12" s="4">
+        <v>100008254</v>
+      </c>
+      <c r="K12">
+        <v>22</v>
+      </c>
+      <c r="M12" s="5">
+        <v>100008254</v>
+      </c>
+      <c r="N12" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>100004467</v>
       </c>
       <c r="D13" s="1">
-        <v>100008254</v>
+        <v>100019875</v>
       </c>
       <c r="E13" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>100019875</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="J13" s="4">
+        <v>100010128</v>
+      </c>
+      <c r="K13">
+        <v>14</v>
+      </c>
+      <c r="M13" s="5">
+        <v>100010128</v>
+      </c>
+      <c r="N13" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="D14" s="1">
-        <v>100010128</v>
+        <v>100020526</v>
       </c>
       <c r="E14" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>100020526</v>
+      </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
+      <c r="J14" s="4">
+        <v>100012200</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="M14" s="5">
+        <v>100012200</v>
+      </c>
+      <c r="N14" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>100004467</v>
       </c>
       <c r="D15" s="1">
+        <v>100071170</v>
+      </c>
+      <c r="E15" s="3">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1">
+        <v>100071170</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="J15" s="4">
         <v>100019875</v>
       </c>
-      <c r="E15" s="3">
+      <c r="K15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M15" s="5">
+        <v>100019875</v>
+      </c>
+      <c r="N15" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>20</v>
       </c>
-      <c r="D16" s="1">
+      <c r="J16" s="4">
         <v>100020526</v>
       </c>
-      <c r="E16" s="3">
+      <c r="K16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M16" s="5">
+        <v>100020526</v>
+      </c>
+      <c r="N16" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>100004819</v>
       </c>
-      <c r="D17" s="1">
+      <c r="J17" s="4">
         <v>100071170</v>
       </c>
-      <c r="E17" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>12</v>
+      </c>
+      <c r="M17" s="5">
+        <v>100071170</v>
+      </c>
+      <c r="N17" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>100005156</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>100007808</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>100008254</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>100010128</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>100012200</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>100019875</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>100020526</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>14</v>
       </c>
@@ -1108,6 +1441,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="J1:K17">
+    <sortCondition ref="J1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>